<commit_message>
Minor updates to 'node_cluster' to aid in better layout drawings.
</commit_message>
<xml_diff>
--- a/models/potable_water_treatment_plant/sysconfig_pwtp_400ML.xlsx
+++ b/models/potable_water_treatment_plant/sysconfig_pwtp_400ML.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="208">
   <si>
     <t>component_type</t>
   </si>
@@ -397,9 +397,6 @@
     <t xml:space="preserve">Coagulation and Flocculation </t>
   </si>
   <si>
-    <t>large_pipe_1</t>
-  </si>
-  <si>
     <t>Ozone Disinfection</t>
   </si>
   <si>
@@ -578,9 +575,6 @@
   </si>
   <si>
     <t>chlorine_tank</t>
-  </si>
-  <si>
-    <t>chlorine_contact</t>
   </si>
   <si>
     <t>pipe_to_clearwell</t>
@@ -696,19 +690,19 @@
     <t>Clearwell Output Connector</t>
   </si>
   <si>
-    <t>Input Pipe</t>
-  </si>
-  <si>
-    <t>DAF Pump</t>
-  </si>
-  <si>
     <t>DAF Connector</t>
   </si>
   <si>
-    <t>Main Feed Pump</t>
-  </si>
-  <si>
-    <t>Power Supply</t>
+    <t>input_pipe_1</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>chlorine_contact_chamber</t>
+  </si>
+  <si>
+    <t>Supply</t>
   </si>
 </sst>
 </file>
@@ -977,13 +971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor rgb="FFCAFB4B"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,7 +1020,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="534">
+  <cellStyleXfs count="538">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1441,6 +1435,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1861,16 +1859,10 @@
     <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="28" fillId="8" borderId="0" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="9" borderId="0" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="9" borderId="3" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="28" fillId="8" borderId="3" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1878,6 +1870,12 @@
     </xf>
     <xf numFmtId="2" fontId="31" fillId="0" borderId="3" xfId="413" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1895,7 +1893,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="534">
+  <cellStyles count="538">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2162,6 +2160,8 @@
     <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="413" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -2429,6 +2429,8 @@
     <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
@@ -2556,14 +2558,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <mruColors>
+      <color rgb="FFCAFB4B"/>
+      <color rgb="FFCAFB46"/>
+      <color rgb="FFCAFB5B"/>
+      <color rgb="FFD7FB00"/>
+      <color rgb="FFBBFB00"/>
+      <color rgb="FFBCF130"/>
+      <color rgb="FFE3EC64"/>
       <color rgb="FFFFD6D9"/>
       <color rgb="FFFFBFC8"/>
       <color rgb="FFFF9FA1"/>
-      <color rgb="FFFF6565"/>
-      <color rgb="FFFF7C80"/>
-      <color rgb="FFFF5050"/>
-      <color rgb="FFFF7D80"/>
-      <color rgb="FF066080"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2843,7 +2847,7 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F12" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2863,7 +2867,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="109" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C1" s="109"/>
       <c r="D1" s="109"/>
@@ -2876,7 +2880,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="108" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" s="109"/>
       <c r="D2" s="109"/>
@@ -2916,7 +2920,7 @@
         <v>76</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="75">
         <v>0.02</v>
@@ -2925,7 +2929,7 @@
         <v>28</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G5" s="77">
         <v>1</v>
@@ -2933,13 +2937,13 @@
     </row>
     <row r="6" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B6" s="74" t="s">
         <v>77</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D6" s="75">
         <v>0.04</v>
@@ -2948,7 +2952,7 @@
         <v>28</v>
       </c>
       <c r="F6" s="74" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G6" s="77">
         <v>1</v>
@@ -2956,13 +2960,13 @@
     </row>
     <row r="7" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D7" s="75">
         <v>4.1000000000000002E-2</v>
@@ -2971,7 +2975,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="74" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="G7" s="77">
         <v>1</v>
@@ -2979,13 +2983,13 @@
     </row>
     <row r="8" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D8" s="75">
         <v>4.1000000000000002E-2</v>
@@ -2994,7 +2998,7 @@
         <v>28</v>
       </c>
       <c r="F8" s="74" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="G8" s="77">
         <v>1</v>
@@ -3002,13 +3006,13 @@
     </row>
     <row r="9" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3017,7 +3021,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="74" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G9" s="77">
         <v>1</v>
@@ -3025,13 +3029,13 @@
     </row>
     <row r="10" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" s="74" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D10" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3040,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="74" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G10" s="77">
         <v>1</v>
@@ -3048,13 +3052,13 @@
     </row>
     <row r="11" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D11" s="75">
         <v>3.3000000000000002E-2</v>
@@ -3063,7 +3067,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="74" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="G11" s="77">
         <v>1</v>
@@ -3071,13 +3075,13 @@
     </row>
     <row r="12" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C12" s="74" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D12" s="75">
         <v>3.3000000000000002E-2</v>
@@ -3086,7 +3090,7 @@
         <v>17</v>
       </c>
       <c r="F12" s="74" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="G12" s="77">
         <v>1</v>
@@ -3094,13 +3098,13 @@
     </row>
     <row r="13" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D13" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3109,7 +3113,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G13" s="77">
         <v>1</v>
@@ -3117,13 +3121,13 @@
     </row>
     <row r="14" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D14" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3132,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G14" s="77">
         <v>1</v>
@@ -3140,13 +3144,13 @@
     </row>
     <row r="15" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D15" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3155,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="F15" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G15" s="77">
         <v>1</v>
@@ -3163,13 +3167,13 @@
     </row>
     <row r="16" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D16" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3178,7 +3182,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G16" s="77">
         <v>1</v>
@@ -3186,13 +3190,13 @@
     </row>
     <row r="17" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D17" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3201,7 +3205,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G17" s="77">
         <v>1</v>
@@ -3209,13 +3213,13 @@
     </row>
     <row r="18" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D18" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3224,7 +3228,7 @@
         <v>2</v>
       </c>
       <c r="F18" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G18" s="77">
         <v>1</v>
@@ -3232,13 +3236,13 @@
     </row>
     <row r="19" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C19" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D19" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3247,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G19" s="77">
         <v>1</v>
@@ -3255,13 +3259,13 @@
     </row>
     <row r="20" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D20" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3270,7 +3274,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G20" s="77">
         <v>1</v>
@@ -3281,7 +3285,7 @@
         <v>78</v>
       </c>
       <c r="B21" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" s="74" t="s">
         <v>118</v>
@@ -3304,7 +3308,7 @@
         <v>79</v>
       </c>
       <c r="B22" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C22" s="74" t="s">
         <v>118</v>
@@ -3327,7 +3331,7 @@
         <v>80</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="74" t="s">
         <v>118</v>
@@ -3350,7 +3354,7 @@
         <v>81</v>
       </c>
       <c r="B24" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C24" s="74" t="s">
         <v>118</v>
@@ -3373,7 +3377,7 @@
         <v>82</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" s="74" t="s">
         <v>118</v>
@@ -3396,7 +3400,7 @@
         <v>83</v>
       </c>
       <c r="B26" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C26" s="74" t="s">
         <v>118</v>
@@ -3419,7 +3423,7 @@
         <v>84</v>
       </c>
       <c r="B27" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27" s="74" t="s">
         <v>118</v>
@@ -3442,7 +3446,7 @@
         <v>85</v>
       </c>
       <c r="B28" s="74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C28" s="74" t="s">
         <v>118</v>
@@ -3465,10 +3469,10 @@
         <v>108</v>
       </c>
       <c r="B29" s="74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="74" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D29" s="75">
         <v>5.0000000000000001E-3</v>
@@ -3477,7 +3481,7 @@
         <v>17</v>
       </c>
       <c r="F29" s="74" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G29" s="77">
         <v>1</v>
@@ -3488,7 +3492,7 @@
         <v>86</v>
       </c>
       <c r="B30" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" s="74" t="s">
         <v>117</v>
@@ -3511,7 +3515,7 @@
         <v>87</v>
       </c>
       <c r="B31" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C31" s="74" t="s">
         <v>117</v>
@@ -3534,7 +3538,7 @@
         <v>88</v>
       </c>
       <c r="B32" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C32" s="74" t="s">
         <v>117</v>
@@ -3557,7 +3561,7 @@
         <v>89</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C33" s="74" t="s">
         <v>117</v>
@@ -3580,7 +3584,7 @@
         <v>90</v>
       </c>
       <c r="B34" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C34" s="74" t="s">
         <v>117</v>
@@ -3603,7 +3607,7 @@
         <v>91</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C35" s="74" t="s">
         <v>117</v>
@@ -3626,7 +3630,7 @@
         <v>92</v>
       </c>
       <c r="B36" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C36" s="74" t="s">
         <v>117</v>
@@ -3649,7 +3653,7 @@
         <v>93</v>
       </c>
       <c r="B37" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="74" t="s">
         <v>117</v>
@@ -3672,10 +3676,10 @@
         <v>94</v>
       </c>
       <c r="B38" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" s="74" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D38" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3684,7 +3688,7 @@
         <v>2</v>
       </c>
       <c r="F38" s="74" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G38" s="77">
         <v>1</v>
@@ -3692,13 +3696,13 @@
     </row>
     <row r="39" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C39" s="74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D39" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3707,7 +3711,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G39" s="77">
         <v>1</v>
@@ -3715,13 +3719,13 @@
     </row>
     <row r="40" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B40" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C40" s="74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D40" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3730,7 +3734,7 @@
         <v>2</v>
       </c>
       <c r="F40" s="74" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G40" s="77">
         <v>1</v>
@@ -3741,10 +3745,10 @@
         <v>95</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C41" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D41" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3753,7 +3757,7 @@
         <v>17</v>
       </c>
       <c r="F41" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G41" s="77">
         <v>1</v>
@@ -3764,10 +3768,10 @@
         <v>96</v>
       </c>
       <c r="B42" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C42" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="75">
         <v>2.5000000000000001E-2</v>
@@ -3776,7 +3780,7 @@
         <v>2</v>
       </c>
       <c r="F42" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G42" s="77">
         <v>1</v>
@@ -3787,10 +3791,10 @@
         <v>97</v>
       </c>
       <c r="B43" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C43" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D43" s="75">
         <v>2.5000000000000001E-2</v>
@@ -3799,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="74" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G43" s="77">
         <v>1</v>
@@ -3810,10 +3814,10 @@
         <v>98</v>
       </c>
       <c r="B44" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C44" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D44" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3822,7 +3826,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G44" s="77">
         <v>1</v>
@@ -3830,13 +3834,13 @@
     </row>
     <row r="45" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B45" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C45" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D45" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3845,7 +3849,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G45" s="77">
         <v>1</v>
@@ -3853,13 +3857,13 @@
     </row>
     <row r="46" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C46" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D46" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3868,7 +3872,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G46" s="77">
         <v>1</v>
@@ -3876,13 +3880,13 @@
     </row>
     <row r="47" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B47" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C47" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D47" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3891,7 +3895,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G47" s="77">
         <v>1</v>
@@ -3899,13 +3903,13 @@
     </row>
     <row r="48" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C48" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D48" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3914,7 +3918,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G48" s="77">
         <v>1</v>
@@ -3922,13 +3926,13 @@
     </row>
     <row r="49" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B49" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C49" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D49" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3937,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="F49" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G49" s="77">
         <v>1</v>
@@ -3945,13 +3949,13 @@
     </row>
     <row r="50" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D50" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3960,7 +3964,7 @@
         <v>2</v>
       </c>
       <c r="F50" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G50" s="77">
         <v>1</v>
@@ -3968,13 +3972,13 @@
     </row>
     <row r="51" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B51" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D51" s="75">
         <v>2.5000000000000001E-3</v>
@@ -3983,7 +3987,7 @@
         <v>2</v>
       </c>
       <c r="F51" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G51" s="77">
         <v>1</v>
@@ -3991,13 +3995,13 @@
     </row>
     <row r="52" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B52" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D52" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4006,7 +4010,7 @@
         <v>2</v>
       </c>
       <c r="F52" s="74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G52" s="77">
         <v>1</v>
@@ -4017,10 +4021,10 @@
         <v>99</v>
       </c>
       <c r="B53" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C53" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D53" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4029,7 +4033,7 @@
         <v>2</v>
       </c>
       <c r="F53" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G53" s="77">
         <v>1</v>
@@ -4040,10 +4044,10 @@
         <v>100</v>
       </c>
       <c r="B54" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C54" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D54" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4052,7 +4056,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G54" s="77">
         <v>1</v>
@@ -4063,10 +4067,10 @@
         <v>101</v>
       </c>
       <c r="B55" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C55" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D55" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4075,7 +4079,7 @@
         <v>2</v>
       </c>
       <c r="F55" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G55" s="77">
         <v>1</v>
@@ -4086,10 +4090,10 @@
         <v>102</v>
       </c>
       <c r="B56" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C56" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D56" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4098,7 +4102,7 @@
         <v>2</v>
       </c>
       <c r="F56" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G56" s="77">
         <v>1</v>
@@ -4109,10 +4113,10 @@
         <v>103</v>
       </c>
       <c r="B57" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C57" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D57" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4121,7 +4125,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G57" s="77">
         <v>1</v>
@@ -4132,10 +4136,10 @@
         <v>104</v>
       </c>
       <c r="B58" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C58" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D58" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4144,7 +4148,7 @@
         <v>2</v>
       </c>
       <c r="F58" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G58" s="77">
         <v>1</v>
@@ -4155,10 +4159,10 @@
         <v>105</v>
       </c>
       <c r="B59" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C59" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D59" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4167,7 +4171,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G59" s="77">
         <v>1</v>
@@ -4178,10 +4182,10 @@
         <v>106</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D60" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4190,7 +4194,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G60" s="77">
         <v>1</v>
@@ -4198,13 +4202,13 @@
     </row>
     <row r="61" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B61" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D61" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4213,7 +4217,7 @@
         <v>2</v>
       </c>
       <c r="F61" s="74" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G61" s="77">
         <v>1</v>
@@ -4221,13 +4225,13 @@
     </row>
     <row r="62" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B62" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C62" s="74" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D62" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4236,7 +4240,7 @@
         <v>2</v>
       </c>
       <c r="F62" s="74" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G62" s="77">
         <v>1</v>
@@ -4244,13 +4248,13 @@
     </row>
     <row r="63" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C63" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" s="75">
         <v>3.3000000000000002E-2</v>
@@ -4259,7 +4263,7 @@
         <v>17</v>
       </c>
       <c r="F63" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G63" s="77">
         <v>1</v>
@@ -4267,13 +4271,13 @@
     </row>
     <row r="64" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B64" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C64" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D64" s="75">
         <v>3.3000000000000002E-2</v>
@@ -4282,7 +4286,7 @@
         <v>17</v>
       </c>
       <c r="F64" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G64" s="77">
         <v>1</v>
@@ -4290,13 +4294,13 @@
     </row>
     <row r="65" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="74" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D65" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4305,7 +4309,7 @@
         <v>2</v>
       </c>
       <c r="F65" s="74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G65" s="77">
         <v>1</v>
@@ -4313,13 +4317,13 @@
     </row>
     <row r="66" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="74" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="C66" s="74" t="s">
         <v>181</v>
-      </c>
-      <c r="B66" s="74" t="s">
-        <v>177</v>
-      </c>
-      <c r="C66" s="74" t="s">
-        <v>183</v>
       </c>
       <c r="D66" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4328,7 +4332,7 @@
         <v>2</v>
       </c>
       <c r="F66" s="74" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G66" s="77">
         <v>1</v>
@@ -4336,13 +4340,13 @@
     </row>
     <row r="67" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B67" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C67" s="74" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D67" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4351,7 +4355,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="74" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G67" s="77">
         <v>1</v>
@@ -4362,10 +4366,10 @@
         <v>109</v>
       </c>
       <c r="B68" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C68" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4374,7 +4378,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="74" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G68" s="77">
         <v>1</v>
@@ -4385,10 +4389,10 @@
         <v>110</v>
       </c>
       <c r="B69" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C69" s="74" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D69" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4397,7 +4401,7 @@
         <v>2</v>
       </c>
       <c r="F69" s="74" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G69" s="77">
         <v>1</v>
@@ -4405,13 +4409,13 @@
     </row>
     <row r="70" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B70" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C70" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D70" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4420,7 +4424,7 @@
         <v>2</v>
       </c>
       <c r="F70" s="74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G70" s="77">
         <v>1</v>
@@ -4428,13 +4432,13 @@
     </row>
     <row r="71" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B71" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C71" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D71" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4443,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="F71" s="74" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G71" s="77">
         <v>1</v>
@@ -4451,13 +4455,13 @@
     </row>
     <row r="72" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="74" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B72" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C72" s="80" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D72" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4466,7 +4470,7 @@
         <v>2</v>
       </c>
       <c r="F72" s="74" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G72" s="77">
         <v>1</v>
@@ -4474,13 +4478,13 @@
     </row>
     <row r="73" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B73" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C73" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D73" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4489,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="F73" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G73" s="77">
         <v>1</v>
@@ -4497,13 +4501,13 @@
     </row>
     <row r="74" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B74" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C74" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D74" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4512,7 +4516,7 @@
         <v>2</v>
       </c>
       <c r="F74" s="74" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G74" s="77">
         <v>1</v>
@@ -4523,10 +4527,10 @@
         <v>111</v>
       </c>
       <c r="B75" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C75" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D75" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4535,7 +4539,7 @@
         <v>2</v>
       </c>
       <c r="F75" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G75" s="77">
         <v>1</v>
@@ -4546,10 +4550,10 @@
         <v>112</v>
       </c>
       <c r="B76" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C76" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D76" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4558,7 +4562,7 @@
         <v>2</v>
       </c>
       <c r="F76" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G76" s="77">
         <v>1</v>
@@ -4569,10 +4573,10 @@
         <v>113</v>
       </c>
       <c r="B77" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C77" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D77" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4581,7 +4585,7 @@
         <v>2</v>
       </c>
       <c r="F77" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G77" s="77">
         <v>1</v>
@@ -4592,10 +4596,10 @@
         <v>114</v>
       </c>
       <c r="B78" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C78" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D78" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4604,7 +4608,7 @@
         <v>2</v>
       </c>
       <c r="F78" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G78" s="77">
         <v>1</v>
@@ -4615,10 +4619,10 @@
         <v>115</v>
       </c>
       <c r="B79" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C79" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D79" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4627,7 +4631,7 @@
         <v>2</v>
       </c>
       <c r="F79" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G79" s="77">
         <v>1</v>
@@ -4638,10 +4642,10 @@
         <v>116</v>
       </c>
       <c r="B80" s="74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C80" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D80" s="75">
         <v>2.5000000000000001E-2</v>
@@ -4650,7 +4654,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G80" s="77">
         <v>1</v>
@@ -4658,13 +4662,13 @@
     </row>
     <row r="81" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" s="74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C81" s="74" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D81" s="75">
         <v>2.5000000000000001E-3</v>
@@ -4673,7 +4677,7 @@
         <v>2</v>
       </c>
       <c r="F81" s="74" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G81" s="77">
         <v>1</v>
@@ -4681,13 +4685,13 @@
     </row>
     <row r="82" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B82" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C82" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D82" s="75">
         <v>3.5000000000000001E-3</v>
@@ -4696,7 +4700,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G82" s="77">
         <v>1</v>
@@ -4704,13 +4708,13 @@
     </row>
     <row r="83" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B83" s="74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C83" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D83" s="75">
         <v>3.5000000000000001E-3</v>
@@ -4719,7 +4723,7 @@
         <v>2</v>
       </c>
       <c r="F83" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G83" s="77">
         <v>1</v>
@@ -4727,13 +4731,13 @@
     </row>
     <row r="84" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B84" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C84" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D84" s="75">
         <v>3.3000000000000002E-2</v>
@@ -4742,7 +4746,7 @@
         <v>17</v>
       </c>
       <c r="F84" s="74" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="G84" s="77">
         <v>1</v>
@@ -4750,13 +4754,13 @@
     </row>
     <row r="85" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B85" s="74" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C85" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D85" s="75">
         <v>3.3000000000000002E-2</v>
@@ -4765,7 +4769,7 @@
         <v>17</v>
       </c>
       <c r="F85" s="74" t="s">
-        <v>132</v>
+        <v>205</v>
       </c>
       <c r="G85" s="77">
         <v>1</v>
@@ -4773,13 +4777,13 @@
     </row>
     <row r="86" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B86" s="74" t="s">
         <v>71</v>
       </c>
       <c r="C86" s="74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D86" s="81">
         <v>4.0000000000000001E-3</v>
@@ -4788,7 +4792,7 @@
         <v>2</v>
       </c>
       <c r="F86" s="74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G86" s="77">
         <v>1</v>
@@ -4796,13 +4800,13 @@
     </row>
     <row r="87" spans="1:7" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B87" s="74" t="s">
         <v>71</v>
       </c>
       <c r="C87" s="74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D87" s="81">
         <v>4.0000000000000001E-3</v>
@@ -4811,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="F87" s="74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G87" s="77">
         <v>1</v>
@@ -4871,8 +4875,8 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B9 B10:B89">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12 B13:B89">
       <formula1>ComponentTypeList</formula1>
     </dataValidation>
   </dataValidations>
@@ -4906,7 +4910,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="108" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="108"/>
       <c r="D1" s="108"/>
@@ -4917,7 +4921,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="108" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C2" s="108"/>
       <c r="D2" s="108"/>
@@ -4940,10 +4944,10 @@
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="85">
         <v>1</v>
@@ -4954,10 +4958,10 @@
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="74" t="s">
         <v>175</v>
-      </c>
-      <c r="B6" s="74" t="s">
-        <v>176</v>
       </c>
       <c r="C6" s="85">
         <v>1</v>
@@ -4971,7 +4975,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="85">
         <v>1</v>
@@ -4982,10 +4986,10 @@
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="85">
         <v>1</v>
@@ -4996,10 +5000,10 @@
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="74" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="C9" s="85">
         <v>1</v>
@@ -5010,10 +5014,10 @@
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="C10" s="85">
         <v>1</v>
@@ -5024,10 +5028,10 @@
     </row>
     <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="C11" s="85">
         <v>1</v>
@@ -5038,10 +5042,10 @@
     </row>
     <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B12" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="85">
         <v>1</v>
@@ -5052,10 +5056,10 @@
     </row>
     <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B13" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C13" s="85">
         <v>1</v>
@@ -5066,10 +5070,10 @@
     </row>
     <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C14" s="85">
         <v>1</v>
@@ -5080,10 +5084,10 @@
     </row>
     <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B15" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15" s="85">
         <v>1</v>
@@ -5094,10 +5098,10 @@
     </row>
     <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C16" s="85">
         <v>1</v>
@@ -5108,10 +5112,10 @@
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B17" s="74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C17" s="85">
         <v>1</v>
@@ -5122,10 +5126,10 @@
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C18" s="85">
         <v>1</v>
@@ -5136,10 +5140,10 @@
     </row>
     <row r="19" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="74" t="s">
-        <v>119</v>
+        <v>204</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C19" s="85">
         <v>1</v>
@@ -5150,7 +5154,7 @@
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="74" t="s">
         <v>78</v>
@@ -5164,7 +5168,7 @@
     </row>
     <row r="21" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="74" t="s">
         <v>79</v>
@@ -5178,7 +5182,7 @@
     </row>
     <row r="22" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="74" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="74" t="s">
         <v>80</v>
@@ -5192,7 +5196,7 @@
     </row>
     <row r="23" spans="1:4" s="87" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="74" t="s">
         <v>81</v>
@@ -5206,7 +5210,7 @@
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="74" t="s">
         <v>82</v>
@@ -5220,7 +5224,7 @@
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" s="74" t="s">
         <v>83</v>
@@ -5234,7 +5238,7 @@
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="74" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B26" s="74" t="s">
         <v>84</v>
@@ -5248,7 +5252,7 @@
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="74" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="74" t="s">
         <v>85</v>
@@ -5601,7 +5605,7 @@
         <v>94</v>
       </c>
       <c r="B52" s="74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C52" s="85">
         <v>1</v>
@@ -5615,7 +5619,7 @@
         <v>94</v>
       </c>
       <c r="B53" s="74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C53" s="85">
         <v>1</v>
@@ -5626,7 +5630,7 @@
     </row>
     <row r="54" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="74" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B54" s="74" t="s">
         <v>96</v>
@@ -5640,7 +5644,7 @@
     </row>
     <row r="55" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B55" s="74" t="s">
         <v>97</v>
@@ -5713,7 +5717,7 @@
         <v>98</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C60" s="85">
         <v>1</v>
@@ -5727,7 +5731,7 @@
         <v>98</v>
       </c>
       <c r="B61" s="74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" s="85">
         <v>1</v>
@@ -5741,7 +5745,7 @@
         <v>98</v>
       </c>
       <c r="B62" s="74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C62" s="85">
         <v>1</v>
@@ -5755,7 +5759,7 @@
         <v>98</v>
       </c>
       <c r="B63" s="74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C63" s="85">
         <v>1</v>
@@ -5769,7 +5773,7 @@
         <v>98</v>
       </c>
       <c r="B64" s="74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C64" s="85">
         <v>1</v>
@@ -5783,7 +5787,7 @@
         <v>98</v>
       </c>
       <c r="B65" s="74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="85">
         <v>1</v>
@@ -5797,7 +5801,7 @@
         <v>98</v>
       </c>
       <c r="B66" s="74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C66" s="85">
         <v>1</v>
@@ -5811,7 +5815,7 @@
         <v>98</v>
       </c>
       <c r="B67" s="74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C67" s="85">
         <v>1</v>
@@ -5822,7 +5826,7 @@
     </row>
     <row r="68" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" s="74" t="s">
         <v>99</v>
@@ -5836,7 +5840,7 @@
     </row>
     <row r="69" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="74" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" s="74" t="s">
         <v>100</v>
@@ -5850,7 +5854,7 @@
     </row>
     <row r="70" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" s="74" t="s">
         <v>101</v>
@@ -5864,7 +5868,7 @@
     </row>
     <row r="71" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="74" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B71" s="74" t="s">
         <v>102</v>
@@ -5878,7 +5882,7 @@
     </row>
     <row r="72" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="74" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B72" s="74" t="s">
         <v>103</v>
@@ -5892,7 +5896,7 @@
     </row>
     <row r="73" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="74" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B73" s="74" t="s">
         <v>104</v>
@@ -5906,7 +5910,7 @@
     </row>
     <row r="74" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" s="74" t="s">
         <v>105</v>
@@ -5920,7 +5924,7 @@
     </row>
     <row r="75" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B75" s="74" t="s">
         <v>106</v>
@@ -5937,7 +5941,7 @@
         <v>99</v>
       </c>
       <c r="B76" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C76" s="85">
         <v>1</v>
@@ -5951,7 +5955,7 @@
         <v>100</v>
       </c>
       <c r="B77" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C77" s="85">
         <v>1</v>
@@ -5965,7 +5969,7 @@
         <v>101</v>
       </c>
       <c r="B78" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C78" s="85">
         <v>1</v>
@@ -5979,7 +5983,7 @@
         <v>102</v>
       </c>
       <c r="B79" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" s="85">
         <v>1</v>
@@ -5993,7 +5997,7 @@
         <v>103</v>
       </c>
       <c r="B80" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C80" s="85">
         <v>1</v>
@@ -6007,7 +6011,7 @@
         <v>104</v>
       </c>
       <c r="B81" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C81" s="85">
         <v>1</v>
@@ -6021,7 +6025,7 @@
         <v>105</v>
       </c>
       <c r="B82" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C82" s="85">
         <v>1</v>
@@ -6035,7 +6039,7 @@
         <v>106</v>
       </c>
       <c r="B83" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C83" s="85">
         <v>1</v>
@@ -6046,10 +6050,10 @@
     </row>
     <row r="84" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" s="74" t="s">
         <v>151</v>
-      </c>
-      <c r="B84" s="74" t="s">
-        <v>152</v>
       </c>
       <c r="C84" s="85">
         <v>1</v>
@@ -6060,10 +6064,10 @@
     </row>
     <row r="85" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B85" s="74" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C85" s="85">
         <v>1</v>
@@ -6074,10 +6078,10 @@
     </row>
     <row r="86" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B86" s="74" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C86" s="85">
         <v>1</v>
@@ -6088,10 +6092,10 @@
     </row>
     <row r="87" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="74" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B87" s="74" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="C87" s="85">
         <v>1</v>
@@ -6102,10 +6106,10 @@
     </row>
     <row r="88" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="74" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B88" s="74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C88" s="85">
         <v>1</v>
@@ -6116,10 +6120,10 @@
     </row>
     <row r="89" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="74" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B89" s="74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C89" s="85">
         <v>1</v>
@@ -6130,7 +6134,7 @@
     </row>
     <row r="90" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B90" s="74" t="s">
         <v>109</v>
@@ -6144,7 +6148,7 @@
     </row>
     <row r="91" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B91" s="74" t="s">
         <v>110</v>
@@ -6161,7 +6165,7 @@
         <v>109</v>
       </c>
       <c r="B92" s="74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C92" s="85">
         <v>1</v>
@@ -6175,7 +6179,7 @@
         <v>110</v>
       </c>
       <c r="B93" s="74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C93" s="85">
         <v>1</v>
@@ -6186,10 +6190,10 @@
     </row>
     <row r="94" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B94" s="74" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C94" s="85">
         <v>1</v>
@@ -6200,10 +6204,10 @@
     </row>
     <row r="95" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" s="74" t="s">
         <v>154</v>
-      </c>
-      <c r="B95" s="74" t="s">
-        <v>155</v>
       </c>
       <c r="C95" s="85">
         <v>1</v>
@@ -6214,10 +6218,10 @@
     </row>
     <row r="96" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B96" s="74" t="s">
         <v>155</v>
-      </c>
-      <c r="B96" s="74" t="s">
-        <v>156</v>
       </c>
       <c r="C96" s="85">
         <v>1</v>
@@ -6228,10 +6232,10 @@
     </row>
     <row r="97" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="74" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B97" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C97" s="85">
         <v>1</v>
@@ -6242,7 +6246,7 @@
     </row>
     <row r="98" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B98" s="74" t="s">
         <v>111</v>
@@ -6256,7 +6260,7 @@
     </row>
     <row r="99" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B99" s="74" t="s">
         <v>112</v>
@@ -6270,7 +6274,7 @@
     </row>
     <row r="100" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B100" s="74" t="s">
         <v>113</v>
@@ -6284,7 +6288,7 @@
     </row>
     <row r="101" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B101" s="74" t="s">
         <v>114</v>
@@ -6298,7 +6302,7 @@
     </row>
     <row r="102" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B102" s="74" t="s">
         <v>115</v>
@@ -6312,7 +6316,7 @@
     </row>
     <row r="103" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B103" s="74" t="s">
         <v>116</v>
@@ -6329,7 +6333,7 @@
         <v>111</v>
       </c>
       <c r="B104" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C104" s="85">
         <v>1</v>
@@ -6343,7 +6347,7 @@
         <v>112</v>
       </c>
       <c r="B105" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C105" s="85">
         <v>1</v>
@@ -6357,7 +6361,7 @@
         <v>113</v>
       </c>
       <c r="B106" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C106" s="85">
         <v>1</v>
@@ -6371,7 +6375,7 @@
         <v>114</v>
       </c>
       <c r="B107" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C107" s="85">
         <v>1</v>
@@ -6385,7 +6389,7 @@
         <v>115</v>
       </c>
       <c r="B108" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C108" s="85">
         <v>1</v>
@@ -6399,7 +6403,7 @@
         <v>116</v>
       </c>
       <c r="B109" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C109" s="85">
         <v>1</v>
@@ -6410,10 +6414,10 @@
     </row>
     <row r="110" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B110" s="74" t="s">
         <v>158</v>
-      </c>
-      <c r="B110" s="74" t="s">
-        <v>159</v>
       </c>
       <c r="C110" s="85">
         <v>1</v>
@@ -6424,10 +6428,10 @@
     </row>
     <row r="111" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B111" s="74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C111" s="85">
         <v>1</v>
@@ -6438,10 +6442,10 @@
     </row>
     <row r="112" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B112" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C112" s="85">
         <v>1</v>
@@ -6452,10 +6456,10 @@
     </row>
     <row r="113" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B113" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C113" s="85">
         <v>1</v>
@@ -6466,10 +6470,10 @@
     </row>
     <row r="114" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="74" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B114" s="74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C114" s="85">
         <v>1</v>
@@ -6480,10 +6484,10 @@
     </row>
     <row r="115" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B115" s="74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C115" s="85">
         <v>1</v>
@@ -6494,10 +6498,10 @@
     </row>
     <row r="116" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="74" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B116" s="74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C116" s="85">
         <v>1</v>
@@ -6508,10 +6512,10 @@
     </row>
     <row r="117" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="74" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B117" s="74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C117" s="85">
         <v>1</v>
@@ -6522,7 +6526,7 @@
     </row>
     <row r="118" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="74" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B118" s="74" t="s">
         <v>15</v>
@@ -6536,7 +6540,7 @@
     </row>
     <row r="119" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="74" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B119" s="74" t="s">
         <v>16</v>
@@ -6579,7 +6583,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6596,7 +6600,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="108" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" s="108"/>
       <c r="D1" s="108"/>
@@ -6619,52 +6623,52 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="107" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="107" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="D4" s="107" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5" s="106">
+        <v>173</v>
+      </c>
+      <c r="B5" s="104">
         <v>50</v>
       </c>
       <c r="C5" s="89">
         <v>1</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="88" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6" s="106">
+        <v>174</v>
+      </c>
+      <c r="B6" s="104">
         <v>50</v>
       </c>
       <c r="C6" s="89">
         <v>1</v>
       </c>
       <c r="D6" s="90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="107">
+      <c r="B7" s="105">
         <v>100</v>
       </c>
       <c r="C7" s="94">
@@ -6722,7 +6726,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="108" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" s="108"/>
       <c r="D1" s="108"/>
@@ -6762,9 +6766,9 @@
         <v>15</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="104">
+        <v>122</v>
+      </c>
+      <c r="C5" s="102">
         <v>200</v>
       </c>
       <c r="D5" s="89">
@@ -6780,9 +6784,9 @@
         <v>16</v>
       </c>
       <c r="B6" s="93" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="105">
+        <v>123</v>
+      </c>
+      <c r="C6" s="103">
         <v>200</v>
       </c>
       <c r="D6" s="94">
@@ -7278,7 +7282,7 @@
     </row>
     <row r="13" spans="1:15" s="33" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>18</v>
@@ -7324,7 +7328,7 @@
     </row>
     <row r="14" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>19</v>
@@ -7370,7 +7374,7 @@
     </row>
     <row r="15" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>20</v>
@@ -7416,7 +7420,7 @@
     </row>
     <row r="16" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>21</v>
@@ -8200,7 +8204,7 @@
     </row>
     <row r="33" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="66" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>18</v>
@@ -8246,7 +8250,7 @@
     </row>
     <row r="34" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>19</v>
@@ -8292,7 +8296,7 @@
     </row>
     <row r="35" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B35" s="21" t="s">
         <v>20</v>
@@ -8338,7 +8342,7 @@
     </row>
     <row r="36" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B36" s="21" t="s">
         <v>21</v>
@@ -8384,7 +8388,7 @@
     </row>
     <row r="37" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="66" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>18</v>
@@ -8430,7 +8434,7 @@
     </row>
     <row r="38" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" s="21" t="s">
         <v>19</v>
@@ -8476,7 +8480,7 @@
     </row>
     <row r="39" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>20</v>
@@ -8522,7 +8526,7 @@
     </row>
     <row r="40" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>21</v>
@@ -8568,7 +8572,7 @@
     </row>
     <row r="41" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>18</v>
@@ -8614,7 +8618,7 @@
     </row>
     <row r="42" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>19</v>
@@ -8660,7 +8664,7 @@
     </row>
     <row r="43" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="21" t="s">
         <v>20</v>
@@ -8706,7 +8710,7 @@
     </row>
     <row r="44" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" s="21" t="s">
         <v>21</v>
@@ -8753,7 +8757,7 @@
     </row>
     <row r="45" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>18</v>
@@ -8799,7 +8803,7 @@
     </row>
     <row r="46" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>19</v>
@@ -8845,7 +8849,7 @@
     </row>
     <row r="47" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" s="21" t="s">
         <v>20</v>
@@ -8891,7 +8895,7 @@
     </row>
     <row r="48" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48" s="21" t="s">
         <v>21</v>
@@ -9123,7 +9127,7 @@
     </row>
     <row r="53" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>18</v>
@@ -9169,7 +9173,7 @@
     </row>
     <row r="54" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>19</v>
@@ -9215,7 +9219,7 @@
     </row>
     <row r="55" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B55" s="21" t="s">
         <v>20</v>
@@ -9261,7 +9265,7 @@
     </row>
     <row r="56" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" s="21" t="s">
         <v>21</v>
@@ -9308,7 +9312,7 @@
     </row>
     <row r="57" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>18</v>
@@ -9354,7 +9358,7 @@
     </row>
     <row r="58" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>19</v>
@@ -9400,7 +9404,7 @@
     </row>
     <row r="59" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>20</v>
@@ -9446,7 +9450,7 @@
     </row>
     <row r="60" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B60" s="34" t="s">
         <v>21</v>
@@ -9678,7 +9682,7 @@
     </row>
     <row r="65" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>18</v>
@@ -9723,7 +9727,7 @@
     </row>
     <row r="66" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B66" s="21" t="s">
         <v>19</v>
@@ -9768,7 +9772,7 @@
     </row>
     <row r="67" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B67" s="21" t="s">
         <v>20</v>
@@ -9813,7 +9817,7 @@
     </row>
     <row r="68" spans="1:15" s="20" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B68" s="34" t="s">
         <v>21</v>
@@ -10804,7 +10808,7 @@
     </row>
     <row r="3" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10814,7 +10818,7 @@
     </row>
     <row r="5" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10854,7 +10858,7 @@
     </row>
     <row r="13" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10884,7 +10888,7 @@
     </row>
     <row r="19" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10899,7 +10903,7 @@
     </row>
     <row r="22" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10914,7 +10918,7 @@
     </row>
     <row r="25" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10924,17 +10928,17 @@
     </row>
     <row r="27" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:1" s="53" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>